<commit_message>
Ergodic Markov Chain - Supervisory component
also fixed the Transition Matrix
</commit_message>
<xml_diff>
--- a/projects/mRubis_Transition_Matrix.xlsx
+++ b/projects/mRubis_Transition_Matrix.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Documents\SVN_Giese\courses\21 WiSe\Probabilistic Models - Modeling, Learning, and Analysis\Projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F5D75998-06B6-4010-BCF3-4E7FF60C95A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F92CCC5-37B0-41C1-8425-B5697C78BE7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="18465" windowHeight="10996" xr2:uid="{FF8088DA-243E-475A-B4D5-21A15437A95B}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="18465" windowHeight="10996" firstSheet="1" activeTab="3" xr2:uid="{FF8088DA-243E-475A-B4D5-21A15437A95B}"/>
   </bookViews>
   <sheets>
     <sheet name="prior_transition_matrix" sheetId="2" r:id="rId1"/>
     <sheet name="mRubis_dependencies" sheetId="3" r:id="rId2"/>
     <sheet name="component_diagram" sheetId="4" r:id="rId3"/>
-    <sheet name="traces" sheetId="5" r:id="rId4"/>
+    <sheet name="comp_diagram with sup comp." sheetId="6" r:id="rId4"/>
+    <sheet name="traces" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -735,17 +736,3489 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>495461</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>74071</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>352664</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>165460</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FA495D6-CBC7-48D8-8A97-6E5CC15E143D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8267861" y="1521871"/>
+          <a:ext cx="1800303" cy="634314"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>Supervisory Component</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>468402</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>179615</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>110247</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D056B78-D2C9-4654-85C0-DF69D02F9DC8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1116102" y="180975"/>
+          <a:ext cx="6835913" cy="4272672"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>607188</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>131619</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>28760</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>109971</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Rectangle 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{565E1CD9-D8B3-4E57-88C1-993D14932480}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7731888" y="312594"/>
+          <a:ext cx="69272" cy="159327"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>28760</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>30308</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>391866</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>4582</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Connector: Elbow 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26FB5B1E-BC74-48EE-9E0E-0B6D090A7A22}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+          <a:stCxn id="5" idx="3"/>
+          <a:endCxn id="17" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7801160" y="392258"/>
+          <a:ext cx="1010806" cy="1060124"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="C00000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>248888</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>57687</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>98924</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>130750</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Connector: Elbow 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B8A5377-3A6C-49DD-9ED3-75B2F76928CE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+          <a:stCxn id="16" idx="1"/>
+          <a:endCxn id="24" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="7871674" y="2379001"/>
+          <a:ext cx="796963" cy="497736"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="C00000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>484226</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>174979</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>643553</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>63276</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Rectangle 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F868C57-4EAD-480F-958C-CB83C7043D32}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="6358554" y="2663601"/>
+          <a:ext cx="69272" cy="159327"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>36080</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>8030</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>427133</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>8651</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Connector: Elbow 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E8BF0A3-52E1-419D-A42E-750B853F577F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+          <a:stCxn id="30" idx="1"/>
+          <a:endCxn id="10" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="9751580" y="1455830"/>
+          <a:ext cx="391053" cy="362571"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector4">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -58458"/>
+            <a:gd name="adj2" fmla="val 175469"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="C00000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>604115</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>8030</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>115742</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>77302</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Rectangle 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E4511F8-2DE0-44B8-AE8F-8498AB8D5B6B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="9716943" y="1410802"/>
+          <a:ext cx="69272" cy="159327"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>221179</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>174325</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>290451</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>152677</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Rectangle 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD45F4C7-8391-4E8B-90BD-199C0F30EE84}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6698179" y="4155775"/>
+          <a:ext cx="69272" cy="159327"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>290451</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>57687</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>414769</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>73014</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="Connector: Elbow 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A36B3731-F654-4C68-B4DF-6515BF1B89ED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+          <a:stCxn id="11" idx="3"/>
+          <a:endCxn id="18" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="6767451" y="2229387"/>
+          <a:ext cx="2067418" cy="2006052"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="C00000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>543297</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>29277</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>495461</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>137281</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Connector: Elbow 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A8C94EC-4550-40C2-9D6F-1473003A2B01}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+          <a:stCxn id="3" idx="1"/>
+          <a:endCxn id="14" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipV="1">
+          <a:off x="5077197" y="1839027"/>
+          <a:ext cx="3190664" cy="650929"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="C00000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>474025</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>57618</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>543297</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>35970</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="Rectangle 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF0F2C8D-5EB9-44A5-BB2A-A4CD01E92530}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5007925" y="2410293"/>
+          <a:ext cx="69272" cy="159327"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>332577</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>16456</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>491904</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>85728</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="Rectangle 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E1AD673-E345-470B-B090-CBA44B6B9BD3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="2968405" y="3228978"/>
+          <a:ext cx="69272" cy="159327"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>19258</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>169391</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>178585</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>57688</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="Rectangle 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{183F5B3F-A12A-46DC-83E5-E68A58C587E3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="8484386" y="2115088"/>
+          <a:ext cx="69272" cy="159327"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>312201</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>4582</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>471528</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>73854</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="Rectangle 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F852E897-AFB2-46EA-BBFD-0EB24F51D921}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="8777329" y="1407354"/>
+          <a:ext cx="69272" cy="159327"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>335104</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>169390</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>494431</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>57687</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="Rectangle 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D9480B3-6D30-4694-9B86-CB12EF93BF7F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="8800232" y="2115087"/>
+          <a:ext cx="69272" cy="159327"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>647021</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>175851</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>158648</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>64148</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="Rectangle 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DDA12747-ADA4-4E9B-8118-72AAAFB435B2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="9112149" y="2121548"/>
+          <a:ext cx="69272" cy="159327"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>466208</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>57619</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>625535</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>126891</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="Rectangle 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA9DA601-0612-44A6-89ED-FDA622A206CE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1806636" y="2365266"/>
+          <a:ext cx="69272" cy="159327"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>79172</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>169389</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>238499</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>57686</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="Rectangle 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2441A780-C888-459E-B163-63494C6AE62C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="9839700" y="2115086"/>
+          <a:ext cx="69272" cy="159327"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>421093</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>111225</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>490365</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>89577</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="Rectangle 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7FBF5DC-9C7B-458F-B7A0-38F127C68B60}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8193493" y="1920975"/>
+          <a:ext cx="69272" cy="159327"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>563891</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>9914</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>421093</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>174979</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="Connector: Elbow 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF4A0D5B-A26A-4D68-A3C6-53C0B8466EBA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+          <a:stCxn id="22" idx="1"/>
+          <a:endCxn id="8" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipV="1">
+          <a:off x="6393191" y="2000639"/>
+          <a:ext cx="1800302" cy="707990"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="C00000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>179615</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>51087</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>248887</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>29439</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name="Rectangle 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CCDA87F-E655-4DC0-A57B-5C73D797CF3B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7952015" y="2946687"/>
+          <a:ext cx="69272" cy="159327"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>338944</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>176316</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>498271</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>64613</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="25" name="Rectangle 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF7B6975-647B-41A6-8A7D-B48858D22CAA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="9451772" y="2122013"/>
+          <a:ext cx="69272" cy="159327"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>474678</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>64148</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>78987</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>70912</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="26" name="Connector: Elbow 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFED609C-DC3A-4FA9-8D3B-3C514BF3D8ED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+          <a:stCxn id="19" idx="1"/>
+          <a:endCxn id="27" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="5431238" y="517788"/>
+          <a:ext cx="1997489" cy="5433609"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 113699"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="C00000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>395013</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>1640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>554340</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>70912</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name="Rectangle 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC266AEA-AC61-4188-A5A5-ED324857E003}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="3678541" y="4119037"/>
+          <a:ext cx="69272" cy="159327"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>412242</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>64612</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>418610</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>85727</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="28" name="Connector: Elbow 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA6E98CD-A164-43D6-A581-73947F3AFD71}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipV="1">
+          <a:off x="3003042" y="2236312"/>
+          <a:ext cx="6483368" cy="1106965"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="C00000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>545872</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>57687</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>158837</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>126892</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="29" name="Connector: Elbow 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B478803D-977B-4F4F-94F6-750D43BF42B8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+          <a:stCxn id="21" idx="1"/>
+          <a:endCxn id="20" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="5732715" y="-1662056"/>
+          <a:ext cx="250180" cy="8033065"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 209372"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="C00000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>357861</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>109963</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>427133</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>88315</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="30" name="Rectangle 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF00B70F-D6F7-44CB-B925-48CA4FC6C473}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="10073361" y="1738738"/>
+          <a:ext cx="69272" cy="159327"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FDC2E87F-D273-4FB8-9061-B42D26F7AC08}" name="Table1" displayName="Table1" ref="B2:E28" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FDC2E87F-D273-4FB8-9061-B42D26F7AC08}" name="Table1" displayName="Table1" ref="B2:E28" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="B2:E28" xr:uid="{AB2A0A11-9B93-4826-B4E6-27F09CCDEBDC}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C3:D28">
     <sortCondition ref="C2:C28"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="3" xr3:uid="{8DBD1A7D-213E-45BF-AF89-F2A64B249D6B}" name="Caller ID" dataDxfId="5"/>
-    <tableColumn id="1" xr3:uid="{A211124B-FE11-42DB-B4F2-460AD6DC516D}" name=" Source (Caller)" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{F99D5DD7-B027-4943-979F-2CE588CB1BCF}" name="Target (Callee)" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{B872D00D-F142-412F-8F2D-D6AF210EE448}" name="Target ID" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{8DBD1A7D-213E-45BF-AF89-F2A64B249D6B}" name="Caller ID" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{A211124B-FE11-42DB-B4F2-460AD6DC516D}" name=" Source (Caller)" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{F99D5DD7-B027-4943-979F-2CE588CB1BCF}" name="Target (Callee)" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{B872D00D-F142-412F-8F2D-D6AF210EE448}" name="Target ID" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1050,7 +4523,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{952B1E20-93B6-41EF-8146-C5757541AA46}">
   <dimension ref="A1:U20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -2302,7 +5775,7 @@
   <dimension ref="B1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2721,6 +6194,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECD6955F-D286-45FF-90C5-C9E062AD3B4B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{925B96D2-EAD7-4B80-B054-41AF1930961D}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>